<commit_message>
customer mit mehr attributen
</commit_message>
<xml_diff>
--- a/Doku/todos.xlsx
+++ b/Doku/todos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\fiae-ls8_9_10a\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A37D09-5BC7-4F36-8B0E-183957B0CC78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A034D9DD-B394-4D8D-9A32-0CDEDF7ADBB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="3000" windowWidth="28800" windowHeight="15195" xr2:uid="{2543FABD-8B82-410E-A2E3-912EBF3C3B43}"/>
+    <workbookView xWindow="1215" yWindow="2655" windowWidth="28800" windowHeight="15195" xr2:uid="{2543FABD-8B82-410E-A2E3-912EBF3C3B43}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>Mitarbeiter</t>
   </si>
   <si>
-    <t>JOBE GmbH</t>
-  </si>
-  <si>
     <t>Simone Musterfrau</t>
   </si>
   <si>
@@ -98,18 +95,12 @@
     <t>DB Anlegen</t>
   </si>
   <si>
-    <t>Schulte OHG</t>
-  </si>
-  <si>
     <t>Max Musterman</t>
   </si>
   <si>
     <t>Login Funktionalität</t>
   </si>
   <si>
-    <t>Jobe GmbH, Schulte OHG</t>
-  </si>
-  <si>
     <t>Webseite gestalten ,Webserver installieren</t>
   </si>
   <si>
@@ -129,6 +120,15 @@
   </si>
   <si>
     <t xml:space="preserve">Max Mustermann (*), Tim Taler </t>
+  </si>
+  <si>
+    <t>JOBE GmbH, Haupstr. 2, 30539 Hannover (trustlevel=1.0)</t>
+  </si>
+  <si>
+    <t>Schulte OHG, Nebenstr. 15b, 31134 Hildesheim (trustlevel=0.8)</t>
+  </si>
+  <si>
+    <t>JOBE GmbH, Haupstr. 2, 30539 Hannover (trustlevel=1.0), Schulte OHG, Nebenstr. 15b, 31134 Hildesheim (trustlevel=0.8)</t>
   </si>
 </sst>
 </file>
@@ -700,7 +700,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E12" sqref="E11:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,7 @@
     <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="1"/>
-    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -725,12 +725,12 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>2</v>
@@ -742,15 +742,15 @@
         <v>3</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>11</v>
@@ -759,15 +759,15 @@
         <v>4</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>12</v>
@@ -776,15 +776,15 @@
         <v>3</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
@@ -793,12 +793,12 @@
         <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -810,12 +810,12 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>7</v>
@@ -827,15 +827,15 @@
         <v>8</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>